<commit_message>
trying to create new variable "TYPE" and updating hours sheet
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>reading articles and investigating data set</t>
+  </si>
+  <si>
+    <t>weekly meeting and playing around with data in R</t>
   </si>
 </sst>
 </file>
@@ -369,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -432,6 +435,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43123</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
more work in R and updating hours sheet
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>weekly meeting and playing around with data in R</t>
+  </si>
+  <si>
+    <t>more R work</t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -446,6 +449,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43123</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
R and updating hours
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>more R work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R </t>
+  </si>
+  <si>
+    <t xml:space="preserve">starting power and sample size calcualtions </t>
   </si>
 </sst>
 </file>
@@ -375,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -460,6 +466,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43132</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43136</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
making power simulation and power function; testing them out
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t xml:space="preserve">starting power and sample size calcualtions </t>
+  </si>
+  <si>
+    <t>R work</t>
+  </si>
+  <si>
+    <t>power simulation; power function</t>
   </si>
 </sst>
 </file>
@@ -381,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -488,6 +494,28 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43144</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43149</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
udating hours; updating power function
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>power simulation; power function</t>
+  </si>
+  <si>
+    <t>weekly meeting; updating power function; started DataCamp on ggplots</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -516,6 +519,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43151</v>
+      </c>
+      <c r="B12">
+        <v>2.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
more ggplots; summarizing data into an excel doc
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>weekly meeting; updating power function; started DataCamp on ggplots</t>
+  </si>
+  <si>
+    <t>R work; data camp class</t>
+  </si>
+  <si>
+    <t>weekly meeting; creating ggplots</t>
+  </si>
+  <si>
+    <t>ggplots; summarizng data</t>
   </si>
 </sst>
 </file>
@@ -390,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -469,7 +478,7 @@
         <v>43123</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -480,7 +489,7 @@
         <v>43132</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -528,6 +537,50 @@
       </c>
       <c r="C12" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43153</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43157</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43165</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>43170</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lots of R work and updating hours
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -81,6 +81,33 @@
   </si>
   <si>
     <t>ggplots; summarizng data</t>
+  </si>
+  <si>
+    <t>meeting and coding</t>
+  </si>
+  <si>
+    <t>coding</t>
+  </si>
+  <si>
+    <t>working on it over break</t>
+  </si>
+  <si>
+    <t>coding and working with ggplot</t>
+  </si>
+  <si>
+    <t>weekly meeting working in R</t>
+  </si>
+  <si>
+    <t>more ggplot stuff</t>
+  </si>
+  <si>
+    <t>last meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">starting report </t>
+  </si>
+  <si>
+    <t xml:space="preserve">working on report </t>
   </si>
 </sst>
 </file>
@@ -116,9 +143,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -583,6 +611,182 @@
         <v>16</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>43172</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43177</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43185</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43187</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>43193</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>43164</v>
+      </c>
+      <c r="B22">
+        <v>2.5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>43200</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>43207</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>43212</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>43214</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>43219</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>43221</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>43226</v>
+      </c>
+      <c r="B29">
+        <v>4.5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>43228</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>43233</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>43244</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>